<commit_message>
Issue 50917: test coverage for assay batch files, assay result file old and new root
</commit_message>
<xml_diff>
--- a/data/AssayImportExport/GenericAssay_Run2.xlsx
+++ b/data/AssayImportExport/GenericAssay_Run2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\labkey\develop\server\testautomation\data\AssayImportExport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/AssayImportExport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DB0C25B-C2DF-48EF-82CC-7A5CFE07626E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6D767-E529-0845-B2DC-E171FB94524F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9570" yWindow="4400" windowWidth="28800" windowHeight="15360" xr2:uid="{BBE25223-6DEB-4901-9B12-061BE6ABF7D8}"/>
+    <workbookView xWindow="5760" yWindow="4400" windowWidth="28800" windowHeight="15360" xr2:uid="{BBE25223-6DEB-4901-9B12-061BE6ABF7D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>participantid</t>
   </si>
@@ -51,6 +40,12 @@
   </si>
   <si>
     <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>resultFileField</t>
+  </si>
+  <si>
+    <t>help.jpg</t>
   </si>
 </sst>
 </file>
@@ -71,11 +66,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,13 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,41 +438,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01DC3F9-E214-4D6B-AF27-19EA3CC6393A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>249318596</v>
       </c>
@@ -491,8 +490,11 @@
       <c r="E2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>249318596</v>
       </c>
@@ -509,7 +511,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>249318596</v>
       </c>
@@ -526,7 +528,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>249320107</v>
       </c>
@@ -543,7 +545,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>249320107</v>
       </c>
@@ -560,7 +562,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>249320127</v>
       </c>
@@ -577,7 +579,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>249320127</v>
       </c>
@@ -594,7 +596,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>249320127</v>
       </c>
@@ -611,7 +613,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>249320127</v>
       </c>
@@ -628,7 +630,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>249320489</v>
       </c>
@@ -645,7 +647,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>249320489</v>
       </c>
@@ -662,7 +664,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>249320489</v>
       </c>
@@ -679,7 +681,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>249320897</v>
       </c>
@@ -696,7 +698,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>249320897</v>
       </c>
@@ -713,7 +715,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>249320897</v>
       </c>
@@ -730,7 +732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>249325717</v>
       </c>
@@ -747,7 +749,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>249325717</v>
       </c>
@@ -764,7 +766,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>249325717</v>
       </c>
@@ -781,7 +783,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>249325717</v>
       </c>
@@ -798,13 +800,13 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B23" s="1"/>
     </row>
   </sheetData>
@@ -820,7 +822,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -834,7 +836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Issue 50917: imported folder archives do not correct file paths for file fields - selenium tests (#2026)
</commit_message>
<xml_diff>
--- a/data/AssayImportExport/GenericAssay_Run2.xlsx
+++ b/data/AssayImportExport/GenericAssay_Run2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\labkey\develop\server\testautomation\data\AssayImportExport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/AssayImportExport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DB0C25B-C2DF-48EF-82CC-7A5CFE07626E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6D767-E529-0845-B2DC-E171FB94524F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9570" yWindow="4400" windowWidth="28800" windowHeight="15360" xr2:uid="{BBE25223-6DEB-4901-9B12-061BE6ABF7D8}"/>
+    <workbookView xWindow="5760" yWindow="4400" windowWidth="28800" windowHeight="15360" xr2:uid="{BBE25223-6DEB-4901-9B12-061BE6ABF7D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>participantid</t>
   </si>
@@ -51,6 +40,12 @@
   </si>
   <si>
     <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>resultFileField</t>
+  </si>
+  <si>
+    <t>help.jpg</t>
   </si>
 </sst>
 </file>
@@ -71,11 +66,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,13 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,41 +438,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01DC3F9-E214-4D6B-AF27-19EA3CC6393A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>249318596</v>
       </c>
@@ -491,8 +490,11 @@
       <c r="E2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>249318596</v>
       </c>
@@ -509,7 +511,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>249318596</v>
       </c>
@@ -526,7 +528,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>249320107</v>
       </c>
@@ -543,7 +545,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>249320107</v>
       </c>
@@ -560,7 +562,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>249320127</v>
       </c>
@@ -577,7 +579,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>249320127</v>
       </c>
@@ -594,7 +596,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>249320127</v>
       </c>
@@ -611,7 +613,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>249320127</v>
       </c>
@@ -628,7 +630,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>249320489</v>
       </c>
@@ -645,7 +647,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>249320489</v>
       </c>
@@ -662,7 +664,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>249320489</v>
       </c>
@@ -679,7 +681,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>249320897</v>
       </c>
@@ -696,7 +698,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>249320897</v>
       </c>
@@ -713,7 +715,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>249320897</v>
       </c>
@@ -730,7 +732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>249325717</v>
       </c>
@@ -747,7 +749,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>249325717</v>
       </c>
@@ -764,7 +766,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>249325717</v>
       </c>
@@ -781,7 +783,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>249325717</v>
       </c>
@@ -798,13 +800,13 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B23" s="1"/>
     </row>
   </sheetData>
@@ -820,7 +822,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -834,7 +836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>